<commit_message>
April 25th update (drop down)
- added visual text selection to dropdown action.
</commit_message>
<xml_diff>
--- a/Test Cases/TestSuite.xlsx
+++ b/Test Cases/TestSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="2670" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="4950" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Test Case XML</t>
   </si>
@@ -68,9 +68,6 @@
     <t>NavigateURL</t>
   </si>
   <si>
-    <t>Step 3</t>
-  </si>
-  <si>
     <t>FunctionName</t>
   </si>
   <si>
@@ -104,13 +101,28 @@
     <t>yes</t>
   </si>
   <si>
+    <t>Validate Mortgage Page</t>
+  </si>
+  <si>
+    <t>https://www.google.ca</t>
+  </si>
+  <si>
+    <t>DropDown</t>
+  </si>
+  <si>
+    <t>//select[@id='landingTerm']</t>
+  </si>
+  <si>
+    <t>Step 5</t>
+  </si>
+  <si>
+    <t>Step 6</t>
+  </si>
+  <si>
     <t>https://tools.td.com/mortgage-payment-calculator/</t>
   </si>
   <si>
-    <t>Validate Mortgage Page</t>
-  </si>
-  <si>
-    <t>DropDown</t>
+    <t>1 Year Open 4%</t>
   </si>
 </sst>
 </file>
@@ -636,13 +648,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -650,13 +662,13 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -664,13 +676,13 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -678,10 +690,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -692,17 +704,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.7109375"/>
     <col min="2" max="2" width="8.5703125"/>
-    <col min="3" max="3" width="23"/>
+    <col min="3" max="3" width="38" customWidth="1"/>
     <col min="4" max="4" width="20.28515625"/>
     <col min="5" max="5" width="21.7109375" style="5"/>
     <col min="6" max="1025" width="8.140625"/>
@@ -727,7 +739,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -736,12 +748,12 @@
         <v>10</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -750,23 +762,43 @@
         <v>12</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
+      <c r="E4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E5" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId2"/>
@@ -793,13 +825,13 @@
   <sheetData>
     <row r="1" spans="1:5" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
5 pm updaate - April 26
</commit_message>
<xml_diff>
--- a/Test Cases/TestSuite.xlsx
+++ b/Test Cases/TestSuite.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="5430" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="4725" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
     <sheet name="Test Cases" sheetId="2" r:id="rId2"/>
     <sheet name="Function" sheetId="3" r:id="rId3"/>
+    <sheet name="Result" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="Action_Keywords">#REF!</definedName>
@@ -18,12 +19,12 @@
     <definedName name="Page_Name">#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A7:D20"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
   <si>
     <t>Test Case XML</t>
   </si>
@@ -200,6 +201,12 @@
   </si>
   <si>
     <t>SCREENSHOT</t>
+  </si>
+  <si>
+    <t>Test case name</t>
+  </si>
+  <si>
+    <t>Result</t>
   </si>
 </sst>
 </file>
@@ -714,10 +721,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,6 +803,17 @@
         <v>23</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -806,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -815,7 +833,7 @@
     <col min="1" max="1" width="51.7109375"/>
     <col min="2" max="2" width="8.5703125"/>
     <col min="3" max="3" width="38" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625"/>
+    <col min="4" max="4" width="32.140625" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" style="5"/>
     <col min="6" max="1025" width="8.140625"/>
   </cols>
@@ -839,7 +857,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -853,7 +871,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -867,7 +885,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -883,8 +901,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="7" t="s">
-        <v>24</v>
+      <c r="A5" t="s">
+        <v>57</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>32</v>
@@ -900,8 +918,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>24</v>
+      <c r="A6" t="s">
+        <v>57</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>28</v>
@@ -917,8 +935,8 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
-        <v>24</v>
+      <c r="A7" t="s">
+        <v>57</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>39</v>
@@ -934,8 +952,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>24</v>
+      <c r="A8" t="s">
+        <v>57</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>45</v>
@@ -951,8 +969,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>24</v>
+      <c r="A9" t="s">
+        <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>46</v>
@@ -966,8 +984,8 @@
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
-        <v>24</v>
+      <c r="A10" t="s">
+        <v>57</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>47</v>
@@ -981,8 +999,8 @@
       <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>24</v>
+      <c r="A11" t="s">
+        <v>57</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>48</v>
@@ -995,7 +1013,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1009,7 +1027,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1023,7 +1041,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
@@ -1040,7 +1058,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>32</v>
@@ -1057,7 +1075,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>28</v>
@@ -1074,7 +1092,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>39</v>
@@ -1091,7 +1109,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>40</v>
@@ -1106,7 +1124,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>41</v>
@@ -1123,7 +1141,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>42</v>
@@ -1140,7 +1158,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>45</v>
@@ -1157,7 +1175,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>46</v>
@@ -1172,7 +1190,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>47</v>
@@ -1189,7 +1207,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>48</v>
@@ -1250,4 +1268,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Documentation Update - April 28th
Added documentation for:
- Header of ActionKeywordsFile
- Documented Click and Navigate actions.
</commit_message>
<xml_diff>
--- a/Test Cases/TestSuite.xlsx
+++ b/Test Cases/TestSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="4725" tabRatio="987" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="16275" windowHeight="4725" tabRatio="987" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <definedName name="Page_Name">#REF!</definedName>
   </definedNames>
   <calcPr calcId="0"/>
-  <oleSize ref="A7:D20"/>
+  <oleSize ref="A1:E13"/>
 </workbook>
 </file>
 
@@ -724,7 +724,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -811,7 +811,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -824,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +857,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -902,7 +902,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>32</v>
@@ -919,7 +919,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B6" s="7" t="s">
         <v>28</v>
@@ -936,7 +936,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B7" s="7" t="s">
         <v>39</v>
@@ -953,7 +953,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>45</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B9" s="7" t="s">
         <v>46</v>
@@ -985,7 +985,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B10" s="7" t="s">
         <v>47</v>
@@ -1000,7 +1000,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
       <c r="B11" s="7" t="s">
         <v>48</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B17" s="7" t="s">
         <v>32</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>28</v>
@@ -1092,7 +1092,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>39</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>40</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>41</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>42</v>
@@ -1158,7 +1158,7 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>45</v>
@@ -1175,7 +1175,7 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>46</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>47</v>
@@ -1207,7 +1207,7 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>57</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>48</v>
@@ -1275,7 +1275,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Resolved "multi catch parameters are not allowed for source level below 1.7"
Changed project compliance to now be at 1.7 instead of 1.5 by default.
Project now doesn't give error on build.
</commit_message>
<xml_diff>
--- a/Test Cases/TestSuite.xlsx
+++ b/Test Cases/TestSuite.xlsx
@@ -18,12 +18,12 @@
     <definedName name="Login_Page">#REF!</definedName>
     <definedName name="Page_Name">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="63">
   <si>
     <t>Test Case XML</t>
   </si>
@@ -211,34 +211,7 @@
     <t>ie</t>
   </si>
   <si>
-    <t>Validate Mortgage Page1</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page2</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page3</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page4</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page5</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page6</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page7</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page8</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page9</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page10</t>
+    <t>.//INPUT[@id='landingAmount']</t>
   </si>
 </sst>
 </file>
@@ -856,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="A29:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -923,7 +896,7 @@
         <v>31</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -1252,137 +1225,40 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>63</v>
-      </c>
-      <c r="B30" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>64</v>
-      </c>
-      <c r="B31" t="s">
-        <v>31</v>
-      </c>
-      <c r="C31" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" t="s">
-        <v>33</v>
-      </c>
-    </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>66</v>
-      </c>
-      <c r="B33" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>67</v>
-      </c>
-      <c r="B34" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C34" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>68</v>
-      </c>
-      <c r="B35" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C36" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>70</v>
-      </c>
-      <c r="B37" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C37" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>71</v>
-      </c>
-      <c r="B38" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+    </row>
+    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
+    </row>
+    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="7"/>
+    </row>
+    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B36" s="7"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="7"/>
+    </row>
+    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="10"/>
+    </row>
+    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="7"/>
       <c r="C38" s="7"/>
-      <c r="D38" s="10" t="s">
-        <v>58</v>
-      </c>
+      <c r="D38" s="10"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Updated test cases to be run
Added Amazon cases to increase case diversity
</commit_message>
<xml_diff>
--- a/Test Cases/TestSuite.xlsx
+++ b/Test Cases/TestSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16275" windowHeight="3795" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15885" windowHeight="3270" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <definedName name="Login_Page">#REF!</definedName>
     <definedName name="Page_Name">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="106">
   <si>
     <t>Test Case XML</t>
   </si>
@@ -190,9 +190,6 @@
     <t>85000.00</t>
   </si>
   <si>
-    <t>Validate With Mahesh</t>
-  </si>
-  <si>
     <t>SCREENSHOT</t>
   </si>
   <si>
@@ -205,29 +202,152 @@
     <t>.//INPUT[@id='landingAmount']</t>
   </si>
   <si>
-    <t>Validate Mortgage Page Firefox</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page temp</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>CLOSEBROWSER</t>
   </si>
   <si>
-    <t>WAIT</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1 </t>
+  </si>
+  <si>
+    <t>CLICK</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/</t>
+  </si>
+  <si>
+    <t>.//INPUT[@id='twotabsearchtextbox']</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>.//SPAN[@class='refinementLink seeMore']</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>(.//img[@id='ebooksImgBlkFront'])</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>.//input[@class='nav-input']</t>
+  </si>
+  <si>
+    <t>(.//span[@class='childRefinementLink'])[4]</t>
+  </si>
+  <si>
+    <t>.//h2[@data-attribute='Selenium WebDriver Practical Guide - Automated Testing for Web Applications']</t>
+  </si>
+  <si>
+    <t>Validate Amazon - Selenium Book</t>
+  </si>
+  <si>
+    <t>Validate Amazon - Shopping Cart</t>
+  </si>
+  <si>
+    <t>.//a[@data-nav-role='signin'][@data-nav-ref='nav_ya_signin']</t>
+  </si>
+  <si>
+    <t>.//input[@type='email']</t>
+  </si>
+  <si>
+    <t>.//input[@type='password']</t>
+  </si>
+  <si>
+    <t>.//input[@id='signInSubmit']</t>
+  </si>
+  <si>
+    <t>seleniumsig</t>
+  </si>
+  <si>
+    <t>seleniumsig@gmail.com</t>
+  </si>
+  <si>
+    <t>Step 14</t>
+  </si>
+  <si>
+    <t>Step 15</t>
+  </si>
+  <si>
+    <t>Step 16</t>
+  </si>
+  <si>
+    <t>TD Bank</t>
+  </si>
+  <si>
+    <t>.//h2[@data-attribute='Banking On America: How TD Bank Rose to the Top and Took on the U.S.A.']</t>
+  </si>
+  <si>
+    <t>.//a[@id='a-autoid-3-announce']</t>
+  </si>
+  <si>
+    <t>.//select[@name='quantity']</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>.//input[@id='bbop-check-box']</t>
+  </si>
+  <si>
+    <t>.//input[@id='add-to-cart-button']</t>
+  </si>
+  <si>
+    <t>.//a[@id='hlb-view-cart-announce']</t>
+  </si>
+  <si>
+    <t>ScreenShot</t>
+  </si>
+  <si>
+    <t>Step 17</t>
+  </si>
+  <si>
+    <t>Step 18</t>
+  </si>
+  <si>
+    <t>Step 19</t>
+  </si>
+  <si>
+    <t>Step 20</t>
+  </si>
+  <si>
+    <t>Step 21</t>
+  </si>
+  <si>
+    <t>TD Bug on Mortgage Page</t>
+  </si>
+  <si>
+    <t>Valiadate Amazon - Empty Cart</t>
+  </si>
+  <si>
+    <t>.//a[@id='nav-cart']</t>
+  </si>
+  <si>
+    <t>.//input[@name='quantityBox']</t>
+  </si>
+  <si>
+    <t>.//a[@id='a-autoid-0-announce']</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>.//input[@aria-label='Delete Banking On America: How Td Bank Rose To The Top And Took On The U']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
@@ -279,6 +399,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -356,7 +482,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -382,6 +508,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -758,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +989,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -859,12 +1000,34 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -874,17 +1037,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.7109375"/>
     <col min="2" max="2" width="8.5703125"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
     <col min="4" max="4" width="32.140625" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" style="5"/>
     <col min="6" max="1025" width="8.140625"/>
@@ -931,7 +1094,7 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -943,13 +1106,13 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,44 +1187,40 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>65</v>
-      </c>
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="B10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>40</v>
+      <c r="B11" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E11" s="8"/>
     </row>
@@ -1070,436 +1229,924 @@
       <c r="C12" s="7"/>
       <c r="E12" s="8"/>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="8"/>
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="9"/>
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="9"/>
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="9"/>
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>27</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
+        <v>74</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>28</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>33</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="8">
-        <v>27</v>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>51</v>
+        <v>75</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>76</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="10"/>
+      <c r="C38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" t="s">
         <v>55</v>
       </c>
-      <c r="B47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="E42" s="9"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="9"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>27</v>
+        <v>10</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>28</v>
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E53" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E54" s="8">
-        <v>5000</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="E55" s="8">
+        <v>5000</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E56" s="8">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E57" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="E57" s="8">
+        <v>27</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E58" s="8">
-        <v>5000</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B59" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E59" s="8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7" t="s">
+      <c r="C60" s="7"/>
+      <c r="D60" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>100</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" t="s">
+        <v>101</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" s="15"/>
+      <c r="D75" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="14"/>
+      <c r="C77" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>100</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E59" r:id="rId1"/>
+    <hyperlink ref="E60" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E29" r:id="rId3"/>
+    <hyperlink ref="E68" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId2"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1549,7 +2196,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,10 +2206,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Testcases updates + minor updates
</commit_message>
<xml_diff>
--- a/Test Cases/TestSuite.xlsx
+++ b/Test Cases/TestSuite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="16275" windowHeight="3795" tabRatio="987"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15885" windowHeight="3270" tabRatio="987"/>
   </bookViews>
   <sheets>
     <sheet name="Test Suite" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <definedName name="Login_Page">#REF!</definedName>
     <definedName name="Page_Name">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="106">
   <si>
     <t>Test Case XML</t>
   </si>
@@ -190,9 +190,6 @@
     <t>85000.00</t>
   </si>
   <si>
-    <t>Validate With Mahesh</t>
-  </si>
-  <si>
     <t>SCREENSHOT</t>
   </si>
   <si>
@@ -205,29 +202,152 @@
     <t>.//INPUT[@id='landingAmount']</t>
   </si>
   <si>
-    <t>Validate Mortgage Page Firefox</t>
-  </si>
-  <si>
-    <t>Validate Mortgage Page temp</t>
-  </si>
-  <si>
-    <t>10000</t>
-  </si>
-  <si>
     <t>CLOSEBROWSER</t>
   </si>
   <si>
-    <t>WAIT</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>0.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step 1 </t>
+  </si>
+  <si>
+    <t>CLICK</t>
+  </si>
+  <si>
+    <t>https://www.amazon.ca/</t>
+  </si>
+  <si>
+    <t>.//INPUT[@id='twotabsearchtextbox']</t>
+  </si>
+  <si>
+    <t>Selenium</t>
+  </si>
+  <si>
+    <t>.//SPAN[@class='refinementLink seeMore']</t>
+  </si>
+  <si>
+    <t>Click</t>
+  </si>
+  <si>
+    <t>(.//img[@id='ebooksImgBlkFront'])</t>
+  </si>
+  <si>
+    <t>wait</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>.//input[@class='nav-input']</t>
+  </si>
+  <si>
+    <t>(.//span[@class='childRefinementLink'])[4]</t>
+  </si>
+  <si>
+    <t>.//h2[@data-attribute='Selenium WebDriver Practical Guide - Automated Testing for Web Applications']</t>
+  </si>
+  <si>
+    <t>Validate Amazon - Selenium Book</t>
+  </si>
+  <si>
+    <t>Validate Amazon - Shopping Cart</t>
+  </si>
+  <si>
+    <t>.//a[@data-nav-role='signin'][@data-nav-ref='nav_ya_signin']</t>
+  </si>
+  <si>
+    <t>.//input[@type='email']</t>
+  </si>
+  <si>
+    <t>.//input[@type='password']</t>
+  </si>
+  <si>
+    <t>.//input[@id='signInSubmit']</t>
+  </si>
+  <si>
+    <t>seleniumsig</t>
+  </si>
+  <si>
+    <t>seleniumsig@gmail.com</t>
+  </si>
+  <si>
+    <t>Step 14</t>
+  </si>
+  <si>
+    <t>Step 15</t>
+  </si>
+  <si>
+    <t>Step 16</t>
+  </si>
+  <si>
+    <t>TD Bank</t>
+  </si>
+  <si>
+    <t>.//h2[@data-attribute='Banking On America: How TD Bank Rose to the Top and Took on the U.S.A.']</t>
+  </si>
+  <si>
+    <t>.//a[@id='a-autoid-3-announce']</t>
+  </si>
+  <si>
+    <t>.//select[@name='quantity']</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>.//input[@id='bbop-check-box']</t>
+  </si>
+  <si>
+    <t>.//input[@id='add-to-cart-button']</t>
+  </si>
+  <si>
+    <t>.//a[@id='hlb-view-cart-announce']</t>
+  </si>
+  <si>
+    <t>ScreenShot</t>
+  </si>
+  <si>
+    <t>Step 17</t>
+  </si>
+  <si>
+    <t>Step 18</t>
+  </si>
+  <si>
+    <t>Step 19</t>
+  </si>
+  <si>
+    <t>Step 20</t>
+  </si>
+  <si>
+    <t>Step 21</t>
+  </si>
+  <si>
+    <t>TD Bug on Mortgage Page</t>
+  </si>
+  <si>
+    <t>Valiadate Amazon - Empty Cart</t>
+  </si>
+  <si>
+    <t>.//a[@id='nav-cart']</t>
+  </si>
+  <si>
+    <t>.//input[@name='quantityBox']</t>
+  </si>
+  <si>
+    <t>.//a[@id='a-autoid-0-announce']</t>
+  </si>
+  <si>
+    <t>Screenshot</t>
+  </si>
+  <si>
+    <t>.//input[@aria-label='Delete Banking On America: How Td Bank Rose To The Top And Took On The U']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF333333"/>
@@ -279,6 +399,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -356,7 +482,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -382,6 +508,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -758,10 +899,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -848,7 +989,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -859,12 +1000,34 @@
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="F7" s="12"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -874,17 +1037,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="51.7109375"/>
     <col min="2" max="2" width="8.5703125"/>
-    <col min="3" max="3" width="38" customWidth="1"/>
+    <col min="3" max="3" width="49.42578125" customWidth="1"/>
     <col min="4" max="4" width="32.140625" customWidth="1"/>
     <col min="5" max="5" width="21.7109375" style="5"/>
     <col min="6" max="1025" width="8.140625"/>
@@ -931,7 +1094,7 @@
       <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="13" t="s">
         <v>27</v>
       </c>
     </row>
@@ -943,13 +1106,13 @@
         <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1024,44 +1187,40 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9" t="s">
-        <v>39</v>
-      </c>
-      <c r="C9" s="7"/>
-      <c r="D9" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>65</v>
-      </c>
+      <c r="B9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="B10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>50</v>
-      </c>
+      <c r="B10" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="D10" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>62</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="E10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
-      <c r="B11" t="s">
-        <v>40</v>
+      <c r="B11" s="7" t="s">
+        <v>44</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E11" s="8"/>
     </row>
@@ -1070,436 +1229,924 @@
       <c r="C12" s="7"/>
       <c r="E12" s="8"/>
     </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>74</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E15" s="8"/>
+      <c r="A15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="9"/>
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>66</v>
+      </c>
+      <c r="D17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="9"/>
+      <c r="A18" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="17"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
-      <c r="E19" s="9"/>
+      <c r="A19" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="16"/>
+      <c r="D19" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>15</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B20" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>27</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B21" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>59</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
+        <v>74</v>
+      </c>
+      <c r="B22" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>28</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="7"/>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="9"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>33</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="B24" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="9"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>35</v>
-      </c>
+      <c r="B25" s="7"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="B26" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="8">
-        <v>27</v>
+      <c r="D26" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>61</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>51</v>
+        <v>75</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>76</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="E28" s="8"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>61</v>
-      </c>
-      <c r="B29" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C32" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>75</v>
+      </c>
+      <c r="B33" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C33" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>75</v>
+      </c>
+      <c r="B34" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="8"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>75</v>
+      </c>
+      <c r="B36" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>75</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E37" s="9"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>75</v>
+      </c>
+      <c r="B38" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C29" s="7"/>
-      <c r="D29" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B34" s="7"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="7"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B36" s="7"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="7"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B38" s="7"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="10"/>
+      <c r="C38" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B39" s="7"/>
-      <c r="C39" s="7"/>
-      <c r="D39" s="10"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="A39" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C39" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="8"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C40" t="s">
+        <v>91</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="C42" s="7"/>
+      <c r="D42" t="s">
         <v>55</v>
       </c>
-      <c r="B47" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="E42" s="9"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>75</v>
+      </c>
+      <c r="B43" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" t="s">
+        <v>36</v>
+      </c>
+      <c r="E43" s="9"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="C44" s="7"/>
+      <c r="D44" t="s">
+        <v>69</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>75</v>
+      </c>
+      <c r="B45" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="7"/>
+      <c r="D45" t="s">
+        <v>93</v>
+      </c>
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>75</v>
+      </c>
+      <c r="B46" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="D46" t="s">
+        <v>59</v>
+      </c>
+      <c r="E46" s="9"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>12</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>27</v>
+        <v>10</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" t="s">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="D49" t="s">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
-      </c>
-      <c r="B50" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C50" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>28</v>
+        <v>99</v>
+      </c>
+      <c r="B50" t="s">
+        <v>29</v>
+      </c>
+      <c r="C50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D50" t="s">
+        <v>31</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C51" s="7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D51" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E51" s="9" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C52" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D52" s="7" t="s">
         <v>24</v>
       </c>
       <c r="E52" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="D53" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E53" s="9"/>
+        <v>24</v>
+      </c>
+      <c r="E53" s="9" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C54" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E54" s="8">
-        <v>5000</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E54" s="9"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C55" s="7" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E55" s="8" t="s">
-        <v>42</v>
+        <v>31</v>
+      </c>
+      <c r="E55" s="8">
+        <v>5000</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C56" s="7" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E56" s="8">
-        <v>27</v>
+        <v>24</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C57" s="7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D57" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E57" s="8"/>
+        <v>31</v>
+      </c>
+      <c r="E57" s="8">
+        <v>27</v>
+      </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C58" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D58" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E58" s="8">
-        <v>5000</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>55</v>
+        <v>99</v>
       </c>
       <c r="B59" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C59" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E59" s="8">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7" t="s">
+      <c r="C60" s="7"/>
+      <c r="D60" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="E59" s="8" t="s">
+      <c r="E60" s="8" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D61" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>100</v>
+      </c>
+      <c r="B65" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="D65" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>100</v>
+      </c>
+      <c r="B66" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>100</v>
+      </c>
+      <c r="B67" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C67" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="E67" s="8"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>100</v>
+      </c>
+      <c r="B68" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E68" s="13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>100</v>
+      </c>
+      <c r="B69" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C69" t="s">
+        <v>78</v>
+      </c>
+      <c r="D69" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E69" s="20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>100</v>
+      </c>
+      <c r="B70" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="C70" t="s">
+        <v>79</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>100</v>
+      </c>
+      <c r="B71" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C71" t="s">
+        <v>101</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>100</v>
+      </c>
+      <c r="B72" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C72" t="s">
+        <v>102</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E72" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>100</v>
+      </c>
+      <c r="B73" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" t="s">
+        <v>103</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>100</v>
+      </c>
+      <c r="B74" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" s="15"/>
+      <c r="D75" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="E75" s="5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>100</v>
+      </c>
+      <c r="B76" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C76" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="D76" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B77" s="14"/>
+      <c r="C77" s="21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D77" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>100</v>
+      </c>
+      <c r="B78" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="D78" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>100</v>
+      </c>
+      <c r="B79" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="D79" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E59" r:id="rId1"/>
+    <hyperlink ref="E60" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E29" r:id="rId3"/>
+    <hyperlink ref="E68" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId2"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1549,7 +2196,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1559,10 +2206,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>